<commit_message>
Reporting issue resolved, new files created
</commit_message>
<xml_diff>
--- a/Evan/Data_Method_3.xlsx
+++ b/Evan/Data_Method_3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jg300416\Documents\MATLAB\DoD\Evan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A33F29-98D1-4A8F-8979-87A9529A2E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB56F675-AA4D-4438-8654-63E33B8886A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4155" yWindow="4155" windowWidth="21600" windowHeight="12735" xr2:uid="{DB4D1D40-A8DA-456B-A30C-81169D4C9387}"/>
   </bookViews>
@@ -517,43 +517,43 @@
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="E2">
-        <v>2.9000000000000001E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="F2">
-        <v>3.2000000000000001E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="G2">
-        <v>3.6999999999999998E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="H2">
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="I2">
-        <v>2.9000000000000001E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="J2">
-        <v>3.2000000000000001E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="K2">
-        <v>3.6999999999999998E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="L2">
-        <v>204.94079600000003</v>
+        <v>154.91485595000003</v>
       </c>
       <c r="M2">
-        <v>204.94079600000003</v>
+        <v>154.91485595000003</v>
       </c>
       <c r="N2">
-        <v>42.911529799999997</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>42.911529799999997</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>264.61029100000002</v>
+        <v>154.91485595000003</v>
       </c>
       <c r="Q2">
-        <v>264.61029100000002</v>
+        <v>154.91485595000003</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -570,43 +570,43 @@
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="E3">
-        <v>5.5E-2</v>
+        <v>0.05</v>
       </c>
       <c r="F3">
-        <v>0.11899999999999999</v>
+        <v>0.05</v>
       </c>
       <c r="G3">
-        <v>0.126</v>
+        <v>0.05</v>
       </c>
       <c r="H3">
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="I3">
-        <v>5.3999999999999999E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="J3">
-        <v>0.11899999999999999</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="K3">
-        <v>0.124</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="L3">
-        <v>760.6964111328125</v>
+        <v>655.23910522460938</v>
       </c>
       <c r="M3">
-        <v>533.90884399414063</v>
+        <v>406.02493286132813</v>
       </c>
       <c r="N3">
-        <v>173.17962646484375</v>
+        <v>0</v>
       </c>
       <c r="O3">
-        <v>126.67465209960938</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>1605.5221557617188</v>
+        <v>655.23910522460938</v>
       </c>
       <c r="Q3">
-        <v>1349.0333557128906</v>
+        <v>406.02493286132813</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -645,31 +645,43 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="E6">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
+      </c>
+      <c r="F6">
+        <v>0.03</v>
+      </c>
+      <c r="G6">
+        <v>0.03</v>
       </c>
       <c r="H6">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="I6">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J6">
-        <v>0.109</v>
+        <v>0.03</v>
       </c>
       <c r="K6">
-        <v>0.11700000000000001</v>
+        <v>0.03</v>
       </c>
       <c r="L6">
-        <v>168.212890625</v>
+        <v>101.98974609375</v>
       </c>
       <c r="M6">
-        <v>168.212890625</v>
+        <v>101.98974609375</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
       </c>
       <c r="O6">
-        <v>98.1903076171875</v>
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>101.98974609375</v>
       </c>
       <c r="Q6">
-        <v>906.1126708984375</v>
+        <v>101.98974609375</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -686,31 +698,43 @@
         <v>1.9E-2</v>
       </c>
       <c r="E7">
-        <v>2.4E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="F7">
-        <v>3.4000000000000002E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="G7">
-        <v>3.9E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="H7">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="I7">
-        <v>6.3E-2</v>
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="J7">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="K7">
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="L7">
-        <v>133.82720947265625</v>
+        <v>0</v>
       </c>
       <c r="M7">
-        <v>792.56820678710938</v>
+        <v>642.8985595703125</v>
       </c>
       <c r="N7">
-        <v>136.74163818359375</v>
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
       </c>
       <c r="P7">
-        <v>561.43951416015625</v>
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>642.8985595703125</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -727,19 +751,19 @@
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="E8">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="H8">
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="I8">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="L8">
-        <v>75.47760009765625</v>
+        <v>23.162841796875</v>
       </c>
       <c r="M8">
-        <v>75.47760009765625</v>
+        <v>23.162841796875</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -756,19 +780,43 @@
         <v>3.9E-2</v>
       </c>
       <c r="E9">
-        <v>5.6000000000000001E-2</v>
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="F9">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="G9">
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="H9">
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="I9">
-        <v>5.6000000000000001E-2</v>
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="J9">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="K9">
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="L9">
-        <v>1401.5579223632813</v>
+        <v>1061.9125366210938</v>
       </c>
       <c r="M9">
-        <v>1448.4405517578125</v>
+        <v>1108.795166015625</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>1061.9125366210938</v>
+      </c>
+      <c r="Q9">
+        <v>1108.795166015625</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -785,43 +833,43 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="E10">
-        <v>2.9000000000000001E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="F10">
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="G10">
-        <v>5.6000000000000001E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="H10">
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="I10">
-        <v>2.9000000000000001E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="J10">
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="K10">
-        <v>5.6000000000000001E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="L10">
-        <v>230.26784261067706</v>
+        <v>81.278483072916657</v>
       </c>
       <c r="M10">
-        <v>230.26784261067706</v>
+        <v>81.278483072916657</v>
       </c>
       <c r="N10">
-        <v>1938.9152526855471</v>
+        <v>1702.3468017578127</v>
       </c>
       <c r="O10">
-        <v>1938.9152526855471</v>
+        <v>1702.3468017578127</v>
       </c>
       <c r="P10">
-        <v>2254.8484802246094</v>
+        <v>2018.2800292968752</v>
       </c>
       <c r="Q10">
-        <v>2254.8484802246094</v>
+        <v>2018.2800292968752</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -838,43 +886,43 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="E11">
-        <v>0.02</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="F11">
-        <v>3.5999999999999997E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="G11">
-        <v>5.7000000000000002E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="H11">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I11">
-        <v>0.02</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="J11">
-        <v>3.5999999999999997E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="K11">
-        <v>5.7000000000000002E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="L11">
-        <v>33.31756591796875</v>
+        <v>0</v>
       </c>
       <c r="M11">
-        <v>33.31756591796875</v>
+        <v>0</v>
       </c>
       <c r="N11">
-        <v>222.01919555664063</v>
+        <v>0</v>
       </c>
       <c r="O11">
-        <v>222.01919555664063</v>
+        <v>0</v>
       </c>
       <c r="P11">
-        <v>335.01815795898438</v>
+        <v>0</v>
       </c>
       <c r="Q11">
-        <v>335.01815795898438</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -891,7 +939,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="E12">
-        <v>0.128</v>
+        <v>0.123</v>
       </c>
       <c r="F12">
         <v>0.13</v>
@@ -900,25 +948,25 @@
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="I12">
-        <v>0.123</v>
+        <v>0.11799999999999999</v>
       </c>
       <c r="J12">
-        <v>0.13900000000000001</v>
+        <v>0.11799999999999999</v>
       </c>
       <c r="K12">
-        <v>0.14599999999999999</v>
+        <v>0.11799999999999999</v>
       </c>
       <c r="L12">
-        <v>6263.8282775878906</v>
+        <v>6190.277099609375</v>
       </c>
       <c r="M12">
-        <v>6165.435791015625</v>
+        <v>6064.1975402832031</v>
       </c>
       <c r="O12">
-        <v>143.2342529296875</v>
+        <v>0</v>
       </c>
       <c r="Q12">
-        <v>6581.9091796875</v>
+        <v>6064.1975402832031</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -935,19 +983,19 @@
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="E13">
-        <v>5.3999999999999999E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="H13">
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="I13">
-        <v>5.5E-2</v>
+        <v>0.05</v>
       </c>
       <c r="L13">
-        <v>3440.2389526367188</v>
+        <v>3052.1621704101563</v>
       </c>
       <c r="M13">
-        <v>3501.1978149414063</v>
+        <v>3160.5300903320313</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -964,43 +1012,43 @@
         <v>3.1E-2</v>
       </c>
       <c r="E14">
-        <v>5.8000000000000003E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="F14">
-        <v>9.6000000000000002E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="G14">
-        <v>0.10100000000000001</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="H14">
         <v>3.1E-2</v>
       </c>
       <c r="I14">
-        <v>5.8000000000000003E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="J14">
-        <v>9.6000000000000002E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="K14">
-        <v>0.10100000000000001</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="L14">
-        <v>3976.74560546875</v>
+        <v>3615.1237487792969</v>
       </c>
       <c r="M14">
-        <v>3976.74560546875</v>
+        <v>3615.1237487792969</v>
       </c>
       <c r="N14">
-        <v>390.0299072265625</v>
+        <v>0</v>
       </c>
       <c r="O14">
-        <v>390.0299072265625</v>
+        <v>0</v>
       </c>
       <c r="P14">
-        <v>5992.8131103515625</v>
+        <v>3615.1237487792969</v>
       </c>
       <c r="Q14">
-        <v>5992.8131103515625</v>
+        <v>3615.1237487792969</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -1017,43 +1065,43 @@
         <v>1.9E-2</v>
       </c>
       <c r="E15">
-        <v>2.9000000000000001E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="F15">
-        <v>3.1E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="G15">
-        <v>3.5999999999999997E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="H15">
         <v>1.9E-2</v>
       </c>
       <c r="I15">
-        <v>2.9000000000000001E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="J15">
-        <v>3.1E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="K15">
-        <v>3.5999999999999997E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="L15">
-        <v>73.79913330078125</v>
+        <v>43.689727783203125</v>
       </c>
       <c r="M15">
-        <v>73.79913330078125</v>
+        <v>43.689727783203125</v>
       </c>
       <c r="N15">
-        <v>28.537750244140625</v>
+        <v>0</v>
       </c>
       <c r="O15">
-        <v>28.537750244140625</v>
+        <v>0</v>
       </c>
       <c r="P15">
-        <v>113.71612548828125</v>
+        <v>43.689727783203125</v>
       </c>
       <c r="Q15">
-        <v>113.71612548828125</v>
+        <v>43.689727783203125</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -1070,43 +1118,43 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="E16">
-        <v>8.1000000000000003E-2</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="F16">
-        <v>0.13300000000000001</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="G16">
-        <v>0.14499999999999999</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="H16">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I16">
-        <v>0.08</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="J16">
-        <v>0.15</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="K16">
-        <v>0.157</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="L16">
-        <v>3398.0255126953125</v>
+        <v>3344.9020385742188</v>
       </c>
       <c r="M16">
-        <v>3391.1590576171875</v>
+        <v>3331.8252563476563</v>
       </c>
       <c r="N16">
-        <v>136.566162109375</v>
+        <v>0</v>
       </c>
       <c r="O16">
-        <v>86.7767333984375</v>
+        <v>0</v>
       </c>
       <c r="P16">
-        <v>3849.4415283203125</v>
+        <v>3344.9020385742188</v>
       </c>
       <c r="Q16">
-        <v>3997.833251953125</v>
+        <v>3331.8252563476563</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -1123,43 +1171,43 @@
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="E17">
-        <v>4.1000000000000002E-2</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="F17">
-        <v>0.109</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="G17">
-        <v>0.114</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="H17">
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="I17">
-        <v>4.1000000000000002E-2</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="J17">
-        <v>0.109</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="K17">
-        <v>0.114</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="L17">
-        <v>2516.4413452148438</v>
+        <v>2188.65966796875</v>
       </c>
       <c r="M17">
-        <v>2516.4413452148438</v>
+        <v>2188.65966796875</v>
       </c>
       <c r="N17">
-        <v>322.57080078125</v>
+        <v>0</v>
       </c>
       <c r="O17">
-        <v>322.57080078125</v>
+        <v>0</v>
       </c>
       <c r="P17">
-        <v>3834.2361450195313</v>
+        <v>2188.65966796875</v>
       </c>
       <c r="Q17">
-        <v>3834.2361450195313</v>
+        <v>2188.65966796875</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -1176,43 +1224,43 @@
         <v>1.6E-2</v>
       </c>
       <c r="E18">
-        <v>8.5000000000000006E-2</v>
+        <v>0.08</v>
       </c>
       <c r="F18">
-        <v>0.105</v>
+        <v>0.08</v>
       </c>
       <c r="G18">
-        <v>0.113</v>
+        <v>0.08</v>
       </c>
       <c r="H18">
         <v>1.6E-2</v>
       </c>
       <c r="I18">
-        <v>8.5000000000000006E-2</v>
+        <v>0.08</v>
       </c>
       <c r="J18">
-        <v>0.127</v>
+        <v>0.08</v>
       </c>
       <c r="K18">
-        <v>0.14099999999999999</v>
+        <v>0.08</v>
       </c>
       <c r="L18">
-        <v>3252.8610229492188</v>
+        <v>3211.9064331054688</v>
       </c>
       <c r="M18">
-        <v>3252.8610229492188</v>
+        <v>3211.9064331054688</v>
       </c>
       <c r="N18">
-        <v>58.441162109375</v>
+        <v>0</v>
       </c>
       <c r="O18">
-        <v>154.327392578125</v>
+        <v>0</v>
       </c>
       <c r="P18">
-        <v>3414.3218994140625</v>
+        <v>3211.9064331054688</v>
       </c>
       <c r="Q18">
-        <v>3652.9083251953125</v>
+        <v>3211.9064331054688</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -1229,43 +1277,43 @@
         <v>9.5000000000000001E-2</v>
       </c>
       <c r="E19">
-        <v>0.10299999999999999</v>
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="F19">
-        <v>0.108</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="G19">
-        <v>0.11700000000000001</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="H19">
         <v>0.109</v>
       </c>
       <c r="I19">
-        <v>0.11600000000000001</v>
+        <v>0.111</v>
       </c>
       <c r="J19">
         <v>0.13900000000000001</v>
       </c>
       <c r="K19">
-        <v>0.14399999999999999</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="L19">
-        <v>2364.6469116210938</v>
+        <v>1070.831298828125</v>
       </c>
       <c r="M19">
-        <v>2587.738037109375</v>
+        <v>813.934326171875</v>
       </c>
       <c r="N19">
-        <v>3066.5435791015625</v>
+        <v>0</v>
       </c>
       <c r="O19">
-        <v>1375.9536743164063</v>
+        <v>0</v>
       </c>
       <c r="P19">
-        <v>5914.8941040039063</v>
+        <v>1330.810546875</v>
       </c>
       <c r="Q19">
-        <v>7640.5792236328125</v>
+        <v>6264.6255493164063</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -1282,43 +1330,43 @@
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="E20">
-        <v>4.3999999999999997E-2</v>
+        <v>3.9E-2</v>
       </c>
       <c r="F20">
-        <v>0.115</v>
+        <v>3.9E-2</v>
       </c>
       <c r="G20">
-        <v>0.126</v>
+        <v>3.9E-2</v>
       </c>
       <c r="H20">
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="I20">
-        <v>4.3999999999999997E-2</v>
+        <v>3.9E-2</v>
       </c>
       <c r="J20">
-        <v>0.115</v>
+        <v>3.9E-2</v>
       </c>
       <c r="K20">
-        <v>0.126</v>
+        <v>3.9E-2</v>
       </c>
       <c r="L20">
-        <v>397.13287353515625</v>
+        <v>265.02227783203125</v>
       </c>
       <c r="M20">
-        <v>397.13287353515625</v>
+        <v>265.02227783203125</v>
       </c>
       <c r="N20">
-        <v>298.4771728515625</v>
+        <v>0</v>
       </c>
       <c r="O20">
-        <v>298.4771728515625</v>
+        <v>0</v>
       </c>
       <c r="P20">
-        <v>1226.7227172851563</v>
+        <v>265.02227783203125</v>
       </c>
       <c r="Q20">
-        <v>1226.7227172851563</v>
+        <v>265.02227783203125</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -1335,43 +1383,43 @@
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="E21">
-        <v>5.2999999999999999E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="F21">
-        <v>5.3999999999999999E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="G21">
-        <v>5.8999999999999997E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="H21">
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="I21">
-        <v>5.1999999999999998E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="J21">
-        <v>0.23799999999999999</v>
+        <v>4.7E-2</v>
       </c>
       <c r="K21">
-        <v>0.245</v>
+        <v>4.7E-2</v>
       </c>
       <c r="L21">
-        <v>3234.0164184570313</v>
+        <v>2932.18994140625</v>
       </c>
       <c r="M21">
-        <v>3189.727783203125</v>
+        <v>2837.3031616210938</v>
       </c>
       <c r="N21">
-        <v>247.9400634765625</v>
+        <v>0</v>
       </c>
       <c r="O21">
-        <v>494.22454833984375</v>
+        <v>0</v>
       </c>
       <c r="P21">
-        <v>3530.9524536132813</v>
+        <v>2932.18994140625</v>
       </c>
       <c r="Q21">
-        <v>7662.8646850585938</v>
+        <v>2837.3031616210938</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -1388,22 +1436,22 @@
         <v>1.6E-2</v>
       </c>
       <c r="I22">
-        <v>2.1999999999999999E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="J22">
-        <v>0.185</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="K22">
-        <v>0.191</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="M22">
-        <v>35.888671875</v>
+        <v>7.1563720703125</v>
       </c>
       <c r="O22">
-        <v>34.90447998046875</v>
+        <v>0</v>
       </c>
       <c r="Q22">
-        <v>713.07373046875</v>
+        <v>7.1563720703125</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -1420,19 +1468,43 @@
         <v>3.1E-2</v>
       </c>
       <c r="E23">
-        <v>7.0000000000000007E-2</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="F23">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="G23">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="H23">
         <v>3.1E-2</v>
       </c>
       <c r="I23">
-        <v>6.9000000000000006E-2</v>
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="J23">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="K23">
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="L23">
-        <v>3905.7388305664063</v>
+        <v>3773.895263671875</v>
       </c>
       <c r="M23">
-        <v>3889.7018432617188</v>
+        <v>3732.5210571289063</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>3773.895263671875</v>
+      </c>
+      <c r="Q23">
+        <v>3732.5210571289063</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -1449,31 +1521,43 @@
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="E24">
-        <v>5.7000000000000002E-2</v>
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="F24">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="G24">
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="H24">
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="I24">
-        <v>0.04</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="J24">
-        <v>4.1000000000000002E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="K24">
-        <v>4.7E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="L24">
-        <v>1124.3133544921875</v>
+        <v>931.58721923828125</v>
       </c>
       <c r="M24">
-        <v>307.47222900390625</v>
+        <v>57.342529296875</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
       </c>
       <c r="O24">
-        <v>297.12677001953125</v>
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>931.58721923828125</v>
       </c>
       <c r="Q24">
-        <v>652.39715576171875</v>
+        <v>57.342529296875</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -1490,43 +1574,43 @@
         <v>2.7E-2</v>
       </c>
       <c r="E25">
-        <v>3.7999999999999999E-2</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="F25">
-        <v>3.9E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="G25">
-        <v>0.06</v>
+        <v>5.5E-2</v>
       </c>
       <c r="H25">
         <v>2.7E-2</v>
       </c>
       <c r="I25">
-        <v>3.7999999999999999E-2</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="J25">
-        <v>3.9E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="K25">
-        <v>0.06</v>
+        <v>5.5E-2</v>
       </c>
       <c r="L25">
-        <v>73.31085205078125</v>
+        <v>43.22052001953125</v>
       </c>
       <c r="M25">
-        <v>73.31085205078125</v>
+        <v>43.22052001953125</v>
       </c>
       <c r="N25">
-        <v>228.515625</v>
+        <v>221.160888671875</v>
       </c>
       <c r="O25">
-        <v>228.515625</v>
+        <v>221.160888671875</v>
       </c>
       <c r="P25">
-        <v>308.78448486328125</v>
+        <v>276.02386474609375</v>
       </c>
       <c r="Q25">
-        <v>308.78448486328125</v>
+        <v>276.02386474609375</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
@@ -1543,43 +1627,43 @@
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="E26">
-        <v>5.6000000000000001E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="F26">
-        <v>0.218</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="G26">
-        <v>0.23</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="H26">
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="I26">
-        <v>5.6000000000000001E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="J26">
-        <v>0.222</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="K26">
-        <v>0.22900000000000001</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="L26">
-        <v>1520.8816528320313</v>
+        <v>1362.7243041992188</v>
       </c>
       <c r="M26">
-        <v>1520.8816528320313</v>
+        <v>1362.7243041992188</v>
       </c>
       <c r="N26">
-        <v>546.2188720703125</v>
+        <v>0</v>
       </c>
       <c r="O26">
-        <v>389.5721435546875</v>
+        <v>0</v>
       </c>
       <c r="P26">
-        <v>3634.2620849609375</v>
+        <v>1362.7243041992188</v>
       </c>
       <c r="Q26">
-        <v>3612.9226684570313</v>
+        <v>1362.7243041992188</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
@@ -1596,19 +1680,31 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="E27">
-        <v>6.5000000000000002E-2</v>
+        <v>0.06</v>
       </c>
       <c r="H27">
         <v>3.1E-2</v>
       </c>
       <c r="I27">
-        <v>6.6000000000000003E-2</v>
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="J27">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="K27">
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="L27">
-        <v>2541.2216186523438</v>
+        <v>2300.1861572265625</v>
       </c>
       <c r="M27">
-        <v>2796.7300415039063</v>
+        <v>2564.3234252929688</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>2564.3234252929688</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -1625,43 +1721,43 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="E28">
-        <v>5.2999999999999999E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="F28">
-        <v>5.3999999999999999E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="G28">
-        <v>0.06</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="H28">
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="I28">
-        <v>5.2999999999999999E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="J28">
-        <v>5.3999999999999999E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="K28">
-        <v>5.8999999999999997E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="L28">
-        <v>4962.7914428710938</v>
+        <v>4629.4708251953125</v>
       </c>
       <c r="M28">
-        <v>4919.189453125</v>
+        <v>4585.8688354492188</v>
       </c>
       <c r="N28">
-        <v>187.1795654296875</v>
+        <v>0</v>
       </c>
       <c r="O28">
-        <v>176.239013671875</v>
+        <v>0</v>
       </c>
       <c r="P28">
-        <v>5184.0667724609375</v>
+        <v>4629.4708251953125</v>
       </c>
       <c r="Q28">
-        <v>5129.5242309570313</v>
+        <v>4585.8688354492188</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -1678,31 +1774,31 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="E29">
-        <v>5.8000000000000003E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="F29">
-        <v>0.14099999999999999</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="G29">
-        <v>0.14899999999999999</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="H29">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="I29">
-        <v>5.6000000000000001E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="L29">
-        <v>1165.5378341674805</v>
+        <v>982.69462585449219</v>
       </c>
       <c r="M29">
-        <v>1112.7138137817383</v>
+        <v>902.68611907958984</v>
       </c>
       <c r="N29">
-        <v>288.848876953125</v>
+        <v>0</v>
       </c>
       <c r="P29">
-        <v>2259.4547271728516</v>
+        <v>982.69462585449219</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -1719,43 +1815,43 @@
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="E30">
-        <v>5.0999999999999997E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="F30">
-        <v>5.2999999999999999E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="G30">
-        <v>9.7000000000000003E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="H30">
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="I30">
-        <v>5.0999999999999997E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="J30">
-        <v>5.1999999999999998E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="K30">
-        <v>9.8000000000000004E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="L30">
-        <v>559.26513671875</v>
+        <v>523.79608154296875</v>
       </c>
       <c r="M30">
-        <v>559.26513671875</v>
+        <v>523.79608154296875</v>
       </c>
       <c r="N30">
-        <v>582.40509033203125</v>
+        <v>0</v>
       </c>
       <c r="O30">
-        <v>595.68023681640625</v>
+        <v>0</v>
       </c>
       <c r="P30">
-        <v>1155.426025390625</v>
+        <v>523.79608154296875</v>
       </c>
       <c r="Q30">
-        <v>1160.2401733398438</v>
+        <v>523.79608154296875</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -1783,43 +1879,43 @@
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="E32">
-        <v>4.3999999999999997E-2</v>
+        <v>3.9E-2</v>
       </c>
       <c r="F32">
-        <v>0.112</v>
+        <v>3.9E-2</v>
       </c>
       <c r="G32">
-        <v>0.11899999999999999</v>
+        <v>3.9E-2</v>
       </c>
       <c r="H32">
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="I32">
-        <v>4.4999999999999998E-2</v>
+        <v>0.04</v>
       </c>
       <c r="J32">
-        <v>0.112</v>
+        <v>0.04</v>
       </c>
       <c r="K32">
-        <v>0.11899999999999999</v>
+        <v>0.04</v>
       </c>
       <c r="L32">
-        <v>64.24713134765625</v>
+        <v>26.06201171875</v>
       </c>
       <c r="M32">
-        <v>70.03021240234375</v>
+        <v>35.2325439453125</v>
       </c>
       <c r="N32">
-        <v>65.460205078125</v>
+        <v>0</v>
       </c>
       <c r="O32">
-        <v>65.460205078125</v>
+        <v>0</v>
       </c>
       <c r="P32">
-        <v>351.75323486328125</v>
+        <v>26.06201171875</v>
       </c>
       <c r="Q32">
-        <v>351.75323486328125</v>
+        <v>35.2325439453125</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
@@ -1836,19 +1932,31 @@
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="E33">
-        <v>4.3999999999999997E-2</v>
+        <v>3.9E-2</v>
+      </c>
+      <c r="F33">
+        <v>0.04</v>
+      </c>
+      <c r="G33">
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="H33">
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="I33">
-        <v>4.2999999999999997E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="L33">
-        <v>98.20556640625</v>
+        <v>63.28582763671875</v>
       </c>
       <c r="M33">
-        <v>92.09442138671875</v>
+        <v>56.34307861328125</v>
+      </c>
+      <c r="N33">
+        <v>7.3089599609375</v>
+      </c>
+      <c r="P33">
+        <v>77.239990234375</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
@@ -1865,19 +1973,43 @@
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="E34">
-        <v>5.5E-2</v>
+        <v>0.05</v>
+      </c>
+      <c r="F34">
+        <v>0.05</v>
+      </c>
+      <c r="G34">
+        <v>0.05</v>
       </c>
       <c r="H34">
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="I34">
-        <v>5.5E-2</v>
+        <v>0.05</v>
+      </c>
+      <c r="J34">
+        <v>0.05</v>
+      </c>
+      <c r="K34">
+        <v>0.05</v>
       </c>
       <c r="L34">
-        <v>6295.654296875</v>
+        <v>5352.783203125</v>
       </c>
       <c r="M34">
-        <v>6295.654296875</v>
+        <v>5352.783203125</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <v>5352.783203125</v>
+      </c>
+      <c r="Q34">
+        <v>5352.783203125</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
@@ -1894,43 +2026,43 @@
         <v>0.04</v>
       </c>
       <c r="E35">
-        <v>5.5E-2</v>
+        <v>0.05</v>
       </c>
       <c r="F35">
-        <v>0.153</v>
+        <v>0.05</v>
       </c>
       <c r="G35">
-        <v>0.16200000000000001</v>
+        <v>0.05</v>
       </c>
       <c r="H35">
         <v>0.04</v>
       </c>
       <c r="I35">
-        <v>5.5E-2</v>
+        <v>0.05</v>
       </c>
       <c r="J35">
-        <v>0.153</v>
+        <v>0.05</v>
       </c>
       <c r="K35">
-        <v>0.16200000000000001</v>
+        <v>0.05</v>
       </c>
       <c r="L35">
-        <v>2090.240478515625</v>
+        <v>1658.660888671875</v>
       </c>
       <c r="M35">
-        <v>2090.240478515625</v>
+        <v>1658.660888671875</v>
       </c>
       <c r="N35">
-        <v>860.19134521484375</v>
+        <v>0</v>
       </c>
       <c r="O35">
-        <v>860.19134521484375</v>
+        <v>0</v>
       </c>
       <c r="P35">
-        <v>5197.8759765625</v>
+        <v>1658.660888671875</v>
       </c>
       <c r="Q35">
-        <v>5197.8759765625</v>
+        <v>1658.660888671875</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
@@ -1947,19 +2079,43 @@
         <v>0.03</v>
       </c>
       <c r="E36">
-        <v>0.06</v>
+        <v>5.5E-2</v>
+      </c>
+      <c r="F36">
+        <v>5.5E-2</v>
+      </c>
+      <c r="G36">
+        <v>5.5E-2</v>
       </c>
       <c r="H36">
         <v>0.03</v>
       </c>
       <c r="I36">
-        <v>6.3E-2</v>
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="J36">
+        <v>0.06</v>
+      </c>
+      <c r="K36">
+        <v>0.06</v>
       </c>
       <c r="L36">
+        <v>1205.108642578125</v>
+      </c>
+      <c r="M36">
+        <v>1303.6117553710938</v>
+      </c>
+      <c r="N36">
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <v>1205.108642578125</v>
+      </c>
+      <c r="Q36">
         <v>1339.6377563476563</v>
-      </c>
-      <c r="M36">
-        <v>1409.5840454101563</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
@@ -1976,31 +2132,43 @@
         <v>0.06</v>
       </c>
       <c r="E37">
-        <v>6.5000000000000002E-2</v>
+        <v>0.06</v>
       </c>
       <c r="F37">
-        <v>7.1999999999999995E-2</v>
+        <v>0.06</v>
       </c>
       <c r="G37">
-        <v>7.6999999999999999E-2</v>
+        <v>0.06</v>
       </c>
       <c r="H37">
         <v>0.124</v>
       </c>
       <c r="I37">
-        <v>0.129</v>
+        <v>0.124</v>
+      </c>
+      <c r="J37">
+        <v>0.124</v>
+      </c>
+      <c r="K37">
+        <v>0.124</v>
       </c>
       <c r="L37">
-        <v>68.634033203125</v>
+        <v>0</v>
       </c>
       <c r="M37">
-        <v>67.108154296875</v>
+        <v>0</v>
       </c>
       <c r="N37">
-        <v>63.94195556640625</v>
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
       </c>
       <c r="P37">
-        <v>209.6710205078125</v>
+        <v>0</v>
+      </c>
+      <c r="Q37">
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
@@ -2017,19 +2185,43 @@
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="E38">
-        <v>0.04</v>
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="F38">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G38">
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="H38">
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="I38">
-        <v>0.04</v>
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="J38">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="K38">
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="L38">
-        <v>52.1240234375</v>
+        <v>11.138916015625</v>
       </c>
       <c r="M38">
-        <v>52.1240234375</v>
+        <v>11.138916015625</v>
+      </c>
+      <c r="N38">
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+      <c r="P38">
+        <v>11.138916015625</v>
+      </c>
+      <c r="Q38">
+        <v>11.138916015625</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -2046,19 +2238,19 @@
         <v>3.9E-2</v>
       </c>
       <c r="E39">
-        <v>5.0999999999999997E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="H39">
         <v>3.9E-2</v>
       </c>
       <c r="I39">
-        <v>5.0999999999999997E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="L39">
-        <v>169.8760986328125</v>
+        <v>113.76190185546875</v>
       </c>
       <c r="M39">
-        <v>169.8760986328125</v>
+        <v>113.76190185546875</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
@@ -2075,19 +2267,43 @@
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="E40">
-        <v>5.2999999999999999E-2</v>
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="F40">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="G40">
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="H40">
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="I40">
-        <v>5.2999999999999999E-2</v>
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="J40">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="K40">
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="L40">
-        <v>3810.1882934570313</v>
+        <v>3570.5337524414063</v>
       </c>
       <c r="M40">
-        <v>3810.1882934570313</v>
+        <v>3570.5337524414063</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+      <c r="P40">
+        <v>3570.5337524414063</v>
+      </c>
+      <c r="Q40">
+        <v>3570.5337524414063</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
@@ -2104,19 +2320,43 @@
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="E41">
-        <v>7.2999999999999995E-2</v>
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="F41">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="G41">
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="H41">
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="I41">
-        <v>7.3999999999999996E-2</v>
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="J41">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="K41">
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="L41">
-        <v>6027.7252197265625</v>
+        <v>5845.1309204101563</v>
       </c>
       <c r="M41">
-        <v>6054.4586181640625</v>
+        <v>5887.9776000976563</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+      <c r="P41">
+        <v>5845.1309204101563</v>
+      </c>
+      <c r="Q41">
+        <v>5887.9776000976563</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
@@ -2133,19 +2373,19 @@
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="E42">
-        <v>4.2999999999999997E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="H42">
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="I42">
-        <v>4.5999999999999999E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="L42">
-        <v>1651.3748168945313</v>
+        <v>1376.2588500976563</v>
       </c>
       <c r="M42">
-        <v>1804.6112060546875</v>
+        <v>1554.4586181640625</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
@@ -2162,43 +2402,43 @@
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="E43">
-        <v>5.8999999999999997E-2</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="F43">
-        <v>0.22600000000000001</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="G43">
-        <v>0.23200000000000001</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="H43">
         <v>0.04</v>
       </c>
       <c r="I43">
-        <v>5.8999999999999997E-2</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="J43">
-        <v>0.185</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="K43">
-        <v>0.19</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="L43">
-        <v>2202.20947265625</v>
+        <v>1767.6162719726563</v>
       </c>
       <c r="M43">
-        <v>2288.848876953125</v>
+        <v>1854.2556762695313</v>
       </c>
       <c r="N43">
-        <v>585.42633056640625</v>
+        <v>0</v>
       </c>
       <c r="O43">
-        <v>374.21417236328125</v>
+        <v>0</v>
       </c>
       <c r="P43">
-        <v>8910.9268188476563</v>
+        <v>1767.6162719726563</v>
       </c>
       <c r="Q43">
-        <v>6326.416015625</v>
+        <v>1854.2556762695313</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
@@ -2215,43 +2455,43 @@
         <v>2.3E-2</v>
       </c>
       <c r="E44">
-        <v>4.2000000000000003E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="F44">
-        <v>5.8000000000000003E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="G44">
-        <v>8.2000000000000003E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="H44">
         <v>2.3E-2</v>
       </c>
       <c r="I44">
-        <v>4.2000000000000003E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="J44">
-        <v>5.8000000000000003E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="K44">
-        <v>8.5999999999999993E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="L44">
-        <v>343.57452392578125</v>
+        <v>295.806884765625</v>
       </c>
       <c r="M44">
-        <v>343.57452392578125</v>
+        <v>295.806884765625</v>
       </c>
       <c r="N44">
-        <v>212.432861328125</v>
+        <v>0</v>
       </c>
       <c r="O44">
-        <v>234.8480224609375</v>
+        <v>0</v>
       </c>
       <c r="P44">
-        <v>623.89373779296875</v>
+        <v>295.806884765625</v>
       </c>
       <c r="Q44">
-        <v>646.30889892578125</v>
+        <v>295.806884765625</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
@@ -2268,43 +2508,43 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="E45">
-        <v>2.9000000000000001E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="F45">
-        <v>0.03</v>
+        <v>2.4E-2</v>
       </c>
       <c r="G45">
-        <v>5.1999999999999998E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="H45">
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="I45">
-        <v>2.9000000000000001E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="J45">
-        <v>0.03</v>
+        <v>2.4E-2</v>
       </c>
       <c r="K45">
-        <v>5.1999999999999998E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="L45">
-        <v>198.02093505859375</v>
+        <v>151.9927978515625</v>
       </c>
       <c r="M45">
-        <v>208.6944580078125</v>
+        <v>162.66632080078125</v>
       </c>
       <c r="N45">
-        <v>559.7381591796875</v>
+        <v>0</v>
       </c>
       <c r="O45">
-        <v>559.7381591796875</v>
+        <v>0</v>
       </c>
       <c r="P45">
-        <v>765.84625244140625</v>
+        <v>151.9927978515625</v>
       </c>
       <c r="Q45">
-        <v>776.519775390625</v>
+        <v>162.66632080078125</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
@@ -2321,19 +2561,43 @@
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="E46">
-        <v>7.1999999999999995E-2</v>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="F46">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="G46">
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="H46">
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="I46">
-        <v>7.1999999999999995E-2</v>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="J46">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="K46">
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="L46">
-        <v>2760.3530883789063</v>
+        <v>2706.756591796875</v>
       </c>
       <c r="M46">
-        <v>2760.3530883789063</v>
+        <v>2706.756591796875</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+      <c r="O46">
+        <v>0</v>
+      </c>
+      <c r="P46">
+        <v>2706.756591796875</v>
+      </c>
+      <c r="Q46">
+        <v>2706.756591796875</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
@@ -2350,43 +2614,43 @@
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="E47">
-        <v>4.9000000000000002E-2</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="F47">
-        <v>0.05</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="G47">
-        <v>5.5E-2</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="H47">
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="I47">
-        <v>4.9000000000000002E-2</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="J47">
-        <v>0.05</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="K47">
-        <v>5.5E-2</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="L47">
-        <v>112.8692626953125</v>
+        <v>0</v>
       </c>
       <c r="M47">
-        <v>112.8692626953125</v>
+        <v>0</v>
       </c>
       <c r="N47">
-        <v>98.65570068359375</v>
+        <v>0</v>
       </c>
       <c r="O47">
-        <v>98.65570068359375</v>
+        <v>0</v>
       </c>
       <c r="P47">
-        <v>231.60552978515625</v>
+        <v>0</v>
       </c>
       <c r="Q47">
-        <v>231.60552978515625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
@@ -2403,19 +2667,31 @@
         <v>6.2E-2</v>
       </c>
       <c r="E48">
-        <v>8.2000000000000003E-2</v>
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="F48">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="G48">
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="H48">
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="I48">
-        <v>8.5000000000000006E-2</v>
+        <v>0.08</v>
       </c>
       <c r="L48">
-        <v>129.96673583984375</v>
+        <v>101.32598876953125</v>
       </c>
       <c r="M48">
-        <v>152.01568603515625</v>
+        <v>125.51116943359375</v>
+      </c>
+      <c r="N48">
+        <v>0</v>
+      </c>
+      <c r="P48">
+        <v>101.32598876953125</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
@@ -2432,43 +2708,43 @@
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="E49">
-        <v>5.2999999999999999E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="F49">
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="G49">
-        <v>6.7000000000000004E-2</v>
+        <v>6.2E-2</v>
       </c>
       <c r="H49">
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="I49">
-        <v>5.2999999999999999E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="J49">
         <v>5.5E-2</v>
       </c>
       <c r="K49">
-        <v>6.7000000000000004E-2</v>
+        <v>6.2E-2</v>
       </c>
       <c r="L49">
-        <v>1383.9492797851563</v>
+        <v>1293.9300537109375</v>
       </c>
       <c r="M49">
-        <v>1383.9492797851563</v>
+        <v>1293.9300537109375</v>
       </c>
       <c r="N49">
-        <v>243.438720703125</v>
+        <v>171.5240478515625</v>
       </c>
       <c r="O49">
-        <v>226.654052734375</v>
+        <v>154.7393798828125</v>
       </c>
       <c r="P49">
-        <v>1641.3803100585938</v>
+        <v>1569.4656372070313</v>
       </c>
       <c r="Q49">
-        <v>1641.3803100585938</v>
+        <v>1569.4656372070313</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
@@ -2496,19 +2772,43 @@
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="E51">
-        <v>5.8999999999999997E-2</v>
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="F51">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="G51">
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="H51">
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="I51">
-        <v>5.8999999999999997E-2</v>
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="J51">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="K51">
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="L51">
-        <v>2098.3428955078125</v>
+        <v>1959.2666625976563</v>
       </c>
       <c r="M51">
-        <v>2098.3428955078125</v>
+        <v>1959.2666625976563</v>
+      </c>
+      <c r="N51">
+        <v>0</v>
+      </c>
+      <c r="O51">
+        <v>0</v>
+      </c>
+      <c r="P51">
+        <v>1959.2666625976563</v>
+      </c>
+      <c r="Q51">
+        <v>1959.2666625976563</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
@@ -2536,43 +2836,43 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="E53">
-        <v>0.06</v>
+        <v>5.5E-2</v>
       </c>
       <c r="F53">
-        <v>6.0999999999999999E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="G53">
-        <v>6.9000000000000006E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="H53">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="I53">
-        <v>0.06</v>
+        <v>5.5E-2</v>
       </c>
       <c r="J53">
-        <v>8.4000000000000005E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="K53">
-        <v>0.113</v>
+        <v>5.5E-2</v>
       </c>
       <c r="L53">
-        <v>4297.2640991210938</v>
+        <v>4064.5904541015625</v>
       </c>
       <c r="M53">
-        <v>4297.2640991210938</v>
+        <v>4064.5904541015625</v>
       </c>
       <c r="N53">
-        <v>354.91180419921875</v>
+        <v>0</v>
       </c>
       <c r="O53">
-        <v>1724.67041015625</v>
+        <v>0</v>
       </c>
       <c r="P53">
-        <v>4704.010009765625</v>
+        <v>4064.5904541015625</v>
       </c>
       <c r="Q53">
-        <v>6828.1097412109375</v>
+        <v>4064.5904541015625</v>
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.25">
@@ -2589,43 +2889,43 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="E54">
-        <v>5.3999999999999999E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="F54">
         <v>6.3E-2</v>
       </c>
       <c r="G54">
-        <v>6.8000000000000005E-2</v>
+        <v>6.3E-2</v>
       </c>
       <c r="H54">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="I54">
-        <v>5.2999999999999999E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="J54">
-        <v>7.6999999999999999E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="K54">
-        <v>8.5000000000000006E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="L54">
-        <v>1537.65869140625</v>
+        <v>1488.7924194335938</v>
       </c>
       <c r="M54">
-        <v>1530.0827026367188</v>
+        <v>1468.1549072265625</v>
       </c>
       <c r="N54">
-        <v>39.61181640625</v>
+        <v>0</v>
       </c>
       <c r="O54">
-        <v>90.01922607421875</v>
+        <v>0</v>
       </c>
       <c r="P54">
-        <v>1641.448974609375</v>
+        <v>1601.837158203125</v>
       </c>
       <c r="Q54">
-        <v>1770.5764770507813</v>
+        <v>1468.1549072265625</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.25">
@@ -2642,43 +2942,43 @@
         <v>3.9E-2</v>
       </c>
       <c r="E55">
-        <v>4.8000000000000001E-2</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="F55">
-        <v>5.5E-2</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="G55">
-        <v>7.0999999999999994E-2</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="H55">
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="I55">
-        <v>6.6000000000000003E-2</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="J55">
-        <v>0.13300000000000001</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="K55">
-        <v>0.13800000000000001</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="L55">
-        <v>237.80059814453125</v>
+        <v>122.0703125</v>
       </c>
       <c r="M55">
-        <v>363.01422119140625</v>
+        <v>202.6519775390625</v>
       </c>
       <c r="N55">
-        <v>538.421630859375</v>
+        <v>0</v>
       </c>
       <c r="O55">
-        <v>158.88214111328125</v>
+        <v>0</v>
       </c>
       <c r="P55">
-        <v>873.17657470703125</v>
+        <v>122.0703125</v>
       </c>
       <c r="Q55">
-        <v>1529.876708984375</v>
+        <v>202.6519775390625</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.25">
@@ -2695,43 +2995,43 @@
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="E56">
-        <v>3.7999999999999999E-2</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="F56">
-        <v>4.1000000000000002E-2</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="G56">
-        <v>5.2999999999999999E-2</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="H56">
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="I56">
-        <v>3.7999999999999999E-2</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="J56">
-        <v>4.1000000000000002E-2</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="K56">
-        <v>5.2999999999999999E-2</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="L56">
-        <v>107.18536376953125</v>
+        <v>74.615478515625</v>
       </c>
       <c r="M56">
-        <v>107.18536376953125</v>
+        <v>74.615478515625</v>
       </c>
       <c r="N56">
-        <v>96.038818359375</v>
+        <v>0</v>
       </c>
       <c r="O56">
-        <v>96.038818359375</v>
+        <v>0</v>
       </c>
       <c r="P56">
-        <v>216.20941162109375</v>
+        <v>74.615478515625</v>
       </c>
       <c r="Q56">
-        <v>216.20941162109375</v>
+        <v>74.615478515625</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.25">
@@ -2748,22 +3048,22 @@
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="I57">
-        <v>3.2000000000000001E-2</v>
+        <v>2.7E-2</v>
       </c>
       <c r="J57">
-        <v>0.05</v>
+        <v>2.7E-2</v>
       </c>
       <c r="K57">
-        <v>5.5E-2</v>
+        <v>2.7E-2</v>
       </c>
       <c r="M57">
-        <v>32.43255615234375</v>
+        <v>6.77490234375</v>
       </c>
       <c r="O57">
-        <v>25.57373046875</v>
+        <v>0</v>
       </c>
       <c r="Q57">
-        <v>110.4278564453125</v>
+        <v>6.77490234375</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
@@ -2780,19 +3080,19 @@
         <v>0.04</v>
       </c>
       <c r="E58">
-        <v>5.1999999999999998E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="H58">
         <v>0.04</v>
       </c>
       <c r="I58">
-        <v>5.1999999999999998E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="L58">
-        <v>667.79327392578125</v>
+        <v>451.3092041015625</v>
       </c>
       <c r="M58">
-        <v>667.79327392578125</v>
+        <v>451.3092041015625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Value call problem resolved
</commit_message>
<xml_diff>
--- a/Evan/Data_Method_3.xlsx
+++ b/Evan/Data_Method_3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jg300416\Documents\MATLAB\DoD\Evan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB56F675-AA4D-4438-8654-63E33B8886A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E94644-3569-4BAC-8209-72E0760281BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4155" yWindow="4155" windowWidth="21600" windowHeight="12735" xr2:uid="{DB4D1D40-A8DA-456B-A30C-81169D4C9387}"/>
   </bookViews>
@@ -517,43 +517,43 @@
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="E2">
-        <v>2.4E-2</v>
+        <v>2.7E-2</v>
       </c>
       <c r="F2">
-        <v>2.4E-2</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="G2">
-        <v>2.4E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="H2">
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="I2">
-        <v>2.4E-2</v>
+        <v>2.7E-2</v>
       </c>
       <c r="J2">
-        <v>2.4E-2</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="K2">
-        <v>2.4E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="L2">
-        <v>154.91485595000003</v>
+        <v>195.74737550000003</v>
       </c>
       <c r="M2">
-        <v>154.91485595000003</v>
+        <v>195.74737550000003</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>28.480529999999998</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>28.480529999999998</v>
       </c>
       <c r="P2">
-        <v>154.91485595000003</v>
+        <v>250.17929120000002</v>
       </c>
       <c r="Q2">
-        <v>154.91485595000003</v>
+        <v>250.17929120000002</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -570,43 +570,43 @@
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="E3">
-        <v>0.05</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="F3">
-        <v>0.05</v>
+        <v>0.11899999999999999</v>
       </c>
       <c r="G3">
-        <v>0.05</v>
+        <v>0.122</v>
       </c>
       <c r="H3">
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="I3">
-        <v>4.9000000000000002E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="J3">
-        <v>4.9000000000000002E-2</v>
+        <v>0.11899999999999999</v>
       </c>
       <c r="K3">
-        <v>4.9000000000000002E-2</v>
+        <v>0.122</v>
       </c>
       <c r="L3">
-        <v>655.23910522460938</v>
+        <v>729.12216186523438</v>
       </c>
       <c r="M3">
-        <v>406.02493286132813</v>
+        <v>501.60598754882813</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>85.895538330078125</v>
       </c>
       <c r="O3">
-        <v>0</v>
+        <v>85.895538330078125</v>
       </c>
       <c r="P3">
-        <v>655.23910522460938</v>
+        <v>1518.2380676269531</v>
       </c>
       <c r="Q3">
-        <v>406.02493286132813</v>
+        <v>1308.2542419433594</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -645,43 +645,31 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="E6">
-        <v>0.03</v>
-      </c>
-      <c r="F6">
-        <v>0.03</v>
-      </c>
-      <c r="G6">
-        <v>0.03</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="H6">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="I6">
-        <v>0.03</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="J6">
-        <v>0.03</v>
+        <v>0.109</v>
       </c>
       <c r="K6">
-        <v>0.03</v>
+        <v>0.114</v>
       </c>
       <c r="L6">
-        <v>101.98974609375</v>
+        <v>154.0069580078125</v>
       </c>
       <c r="M6">
-        <v>101.98974609375</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
+        <v>154.0069580078125</v>
       </c>
       <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>101.98974609375</v>
+        <v>63.7969970703125</v>
       </c>
       <c r="Q6">
-        <v>101.98974609375</v>
+        <v>871.7193603515625</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -698,43 +686,31 @@
         <v>1.9E-2</v>
       </c>
       <c r="E7">
-        <v>1.9E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="F7">
-        <v>1.9E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="G7">
-        <v>1.9E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="H7">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="I7">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="J7">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="K7">
-        <v>5.8000000000000003E-2</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>88.56964111328125</v>
       </c>
       <c r="M7">
-        <v>642.8985595703125</v>
+        <v>748.19183349609375</v>
       </c>
       <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
+        <v>99.582672119140625</v>
       </c>
       <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>642.8985595703125</v>
+        <v>524.28054809570313</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -751,19 +727,19 @@
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="E8">
-        <v>0.03</v>
+        <v>3.1E-2</v>
       </c>
       <c r="H8">
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="I8">
-        <v>0.03</v>
+        <v>3.1E-2</v>
       </c>
       <c r="L8">
-        <v>23.162841796875</v>
+        <v>33.33282470703125</v>
       </c>
       <c r="M8">
-        <v>23.162841796875</v>
+        <v>33.33282470703125</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -780,43 +756,19 @@
         <v>3.9E-2</v>
       </c>
       <c r="E9">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="F9">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="G9">
-        <v>5.0999999999999997E-2</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="H9">
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="I9">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="J9">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="K9">
-        <v>5.0999999999999997E-2</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="L9">
-        <v>1061.9125366210938</v>
+        <v>1333.9080810546875</v>
       </c>
       <c r="M9">
-        <v>1108.795166015625</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <v>1061.9125366210938</v>
-      </c>
-      <c r="Q9">
-        <v>1108.795166015625</v>
+        <v>1380.7907104492188</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -833,43 +785,43 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="E10">
-        <v>2.4E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="F10">
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="G10">
-        <v>5.0999999999999997E-2</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="H10">
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="I10">
-        <v>2.4E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="J10">
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="K10">
-        <v>5.0999999999999997E-2</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="L10">
-        <v>81.278483072916657</v>
+        <v>147.15830485026041</v>
       </c>
       <c r="M10">
-        <v>81.278483072916657</v>
+        <v>147.15830485026041</v>
       </c>
       <c r="N10">
-        <v>1702.3468017578127</v>
+        <v>1900.2978006998701</v>
       </c>
       <c r="O10">
-        <v>1702.3468017578127</v>
+        <v>1900.2978006998701</v>
       </c>
       <c r="P10">
-        <v>2018.2800292968752</v>
+        <v>2216.2310282389321</v>
       </c>
       <c r="Q10">
-        <v>2018.2800292968752</v>
+        <v>2216.2310282389321</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -886,43 +838,43 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="E11">
-        <v>1.4999999999999999E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="F11">
-        <v>1.4999999999999999E-2</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="G11">
-        <v>1.4999999999999999E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="H11">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I11">
-        <v>1.4999999999999999E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="J11">
-        <v>1.4999999999999999E-2</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="K11">
-        <v>1.4999999999999999E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>23.281097412109375</v>
       </c>
       <c r="M11">
-        <v>0</v>
+        <v>23.281097412109375</v>
       </c>
       <c r="N11">
-        <v>0</v>
+        <v>210.16693115234375</v>
       </c>
       <c r="O11">
-        <v>0</v>
+        <v>210.16693115234375</v>
       </c>
       <c r="P11">
-        <v>0</v>
+        <v>323.1658935546875</v>
       </c>
       <c r="Q11">
-        <v>0</v>
+        <v>323.1658935546875</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -939,7 +891,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="E12">
-        <v>0.123</v>
+        <v>0.125</v>
       </c>
       <c r="F12">
         <v>0.13</v>
@@ -948,25 +900,25 @@
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="I12">
-        <v>0.11799999999999999</v>
+        <v>0.121</v>
       </c>
       <c r="J12">
-        <v>0.11799999999999999</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="K12">
-        <v>0.11799999999999999</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="L12">
-        <v>6190.277099609375</v>
+        <v>6219.940185546875</v>
       </c>
       <c r="M12">
-        <v>6064.1975402832031</v>
+        <v>6134.4261169433594</v>
       </c>
       <c r="O12">
-        <v>0</v>
+        <v>104.75540161132813</v>
       </c>
       <c r="Q12">
-        <v>6064.1975402832031</v>
+        <v>6543.4303283691406</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -983,19 +935,19 @@
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="E13">
-        <v>4.9000000000000002E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="H13">
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="I13">
-        <v>0.05</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="L13">
-        <v>3052.1621704101563</v>
+        <v>3239.07470703125</v>
       </c>
       <c r="M13">
-        <v>3160.5300903320313</v>
+        <v>3239.07470703125</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -1012,43 +964,43 @@
         <v>3.1E-2</v>
       </c>
       <c r="E14">
-        <v>5.2999999999999999E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="F14">
-        <v>5.2999999999999999E-2</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="G14">
-        <v>5.2999999999999999E-2</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="H14">
         <v>3.1E-2</v>
       </c>
       <c r="I14">
-        <v>5.2999999999999999E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="J14">
-        <v>5.2999999999999999E-2</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="K14">
-        <v>5.2999999999999999E-2</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="L14">
-        <v>3615.1237487792969</v>
+        <v>3880.0315856933594</v>
       </c>
       <c r="M14">
-        <v>3615.1237487792969</v>
+        <v>3880.0315856933594</v>
       </c>
       <c r="N14">
-        <v>0</v>
+        <v>285.88485717773438</v>
       </c>
       <c r="O14">
-        <v>0</v>
+        <v>285.88485717773438</v>
       </c>
       <c r="P14">
-        <v>3615.1237487792969</v>
+        <v>5888.6680603027344</v>
       </c>
       <c r="Q14">
-        <v>3615.1237487792969</v>
+        <v>5888.6680603027344</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -1065,43 +1017,43 @@
         <v>1.9E-2</v>
       </c>
       <c r="E15">
-        <v>2.4E-2</v>
+        <v>2.7E-2</v>
       </c>
       <c r="F15">
-        <v>2.4E-2</v>
+        <v>3.1E-2</v>
       </c>
       <c r="G15">
-        <v>2.4E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="H15">
         <v>1.9E-2</v>
       </c>
       <c r="I15">
-        <v>2.4E-2</v>
+        <v>2.7E-2</v>
       </c>
       <c r="J15">
-        <v>2.4E-2</v>
+        <v>3.1E-2</v>
       </c>
       <c r="K15">
-        <v>2.4E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="L15">
-        <v>43.689727783203125</v>
+        <v>67.081451416015625</v>
       </c>
       <c r="M15">
-        <v>43.689727783203125</v>
+        <v>67.081451416015625</v>
       </c>
       <c r="N15">
-        <v>0</v>
+        <v>21.4996337890625</v>
       </c>
       <c r="O15">
-        <v>0</v>
+        <v>21.4996337890625</v>
       </c>
       <c r="P15">
-        <v>43.689727783203125</v>
+        <v>106.67800903320313</v>
       </c>
       <c r="Q15">
-        <v>43.689727783203125</v>
+        <v>106.67800903320313</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -1118,43 +1070,43 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="E16">
-        <v>7.5999999999999998E-2</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="F16">
-        <v>7.5999999999999998E-2</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="G16">
-        <v>7.5999999999999998E-2</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="H16">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I16">
-        <v>7.4999999999999997E-2</v>
+        <v>7.8E-2</v>
       </c>
       <c r="J16">
-        <v>7.4999999999999997E-2</v>
+        <v>0.15</v>
       </c>
       <c r="K16">
-        <v>7.4999999999999997E-2</v>
+        <v>0.155</v>
       </c>
       <c r="L16">
-        <v>3344.9020385742188</v>
+        <v>3382.4539184570313</v>
       </c>
       <c r="M16">
-        <v>3331.8252563476563</v>
+        <v>3371.8414306640625</v>
       </c>
       <c r="N16">
-        <v>0</v>
+        <v>118.3624267578125</v>
       </c>
       <c r="O16">
-        <v>0</v>
+        <v>65.8111572265625</v>
       </c>
       <c r="P16">
-        <v>3344.9020385742188</v>
+        <v>3831.23779296875</v>
       </c>
       <c r="Q16">
-        <v>3331.8252563476563</v>
+        <v>3976.86767578125</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -1171,43 +1123,43 @@
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="E17">
-        <v>3.5999999999999997E-2</v>
+        <v>3.9E-2</v>
       </c>
       <c r="F17">
-        <v>3.5999999999999997E-2</v>
+        <v>0.109</v>
       </c>
       <c r="G17">
-        <v>3.5999999999999997E-2</v>
+        <v>0.112</v>
       </c>
       <c r="H17">
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="I17">
-        <v>3.5999999999999997E-2</v>
+        <v>3.9E-2</v>
       </c>
       <c r="J17">
-        <v>3.5999999999999997E-2</v>
+        <v>0.109</v>
       </c>
       <c r="K17">
-        <v>3.5999999999999997E-2</v>
+        <v>0.112</v>
       </c>
       <c r="L17">
-        <v>2188.65966796875</v>
+        <v>2429.5578002929688</v>
       </c>
       <c r="M17">
-        <v>2188.65966796875</v>
+        <v>2429.5578002929688</v>
       </c>
       <c r="N17">
-        <v>0</v>
+        <v>215.61431884765625</v>
       </c>
       <c r="O17">
-        <v>0</v>
+        <v>215.61431884765625</v>
       </c>
       <c r="P17">
-        <v>2188.65966796875</v>
+        <v>3727.2796630859375</v>
       </c>
       <c r="Q17">
-        <v>2188.65966796875</v>
+        <v>3727.2796630859375</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -1224,43 +1176,43 @@
         <v>1.6E-2</v>
       </c>
       <c r="E18">
-        <v>0.08</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="F18">
-        <v>0.08</v>
+        <v>0.105</v>
       </c>
       <c r="G18">
-        <v>0.08</v>
+        <v>0.111</v>
       </c>
       <c r="H18">
         <v>1.6E-2</v>
       </c>
       <c r="I18">
-        <v>0.08</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="J18">
-        <v>0.08</v>
+        <v>0.127</v>
       </c>
       <c r="K18">
-        <v>0.08</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="L18">
-        <v>3211.9064331054688</v>
+        <v>3245.17822265625</v>
       </c>
       <c r="M18">
-        <v>3211.9064331054688</v>
+        <v>3245.17822265625</v>
       </c>
       <c r="N18">
-        <v>0</v>
+        <v>50.14801025390625</v>
       </c>
       <c r="O18">
-        <v>0</v>
+        <v>149.00970458984375</v>
       </c>
       <c r="P18">
-        <v>3211.9064331054688</v>
+        <v>3406.0287475585938</v>
       </c>
       <c r="Q18">
-        <v>3211.9064331054688</v>
+        <v>3647.5906372070313</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -1277,43 +1229,43 @@
         <v>9.5000000000000001E-2</v>
       </c>
       <c r="E19">
-        <v>9.8000000000000004E-2</v>
+        <v>0.10199999999999999</v>
       </c>
       <c r="F19">
-        <v>9.9000000000000005E-2</v>
+        <v>0.108</v>
       </c>
       <c r="G19">
-        <v>9.9000000000000005E-2</v>
+        <v>0.11700000000000001</v>
       </c>
       <c r="H19">
         <v>0.109</v>
       </c>
       <c r="I19">
-        <v>0.111</v>
+        <v>0.112</v>
       </c>
       <c r="J19">
         <v>0.13900000000000001</v>
       </c>
       <c r="K19">
-        <v>0.13900000000000001</v>
+        <v>0.14199999999999999</v>
       </c>
       <c r="L19">
-        <v>1070.831298828125</v>
+        <v>2208.1298828125</v>
       </c>
       <c r="M19">
-        <v>813.934326171875</v>
+        <v>1135.2310180664063</v>
       </c>
       <c r="N19">
-        <v>0</v>
+        <v>3066.5435791015625</v>
       </c>
       <c r="O19">
-        <v>0</v>
+        <v>1059.1278076171875</v>
       </c>
       <c r="P19">
-        <v>1330.810546875</v>
+        <v>5914.8941040039063</v>
       </c>
       <c r="Q19">
-        <v>6264.6255493164063</v>
+        <v>7323.7533569335938</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -1330,43 +1282,43 @@
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="E20">
-        <v>3.9E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="F20">
-        <v>3.9E-2</v>
+        <v>0.115</v>
       </c>
       <c r="G20">
-        <v>3.9E-2</v>
+        <v>0.122</v>
       </c>
       <c r="H20">
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="I20">
-        <v>3.9E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="J20">
-        <v>3.9E-2</v>
+        <v>0.115</v>
       </c>
       <c r="K20">
-        <v>3.9E-2</v>
+        <v>0.122</v>
       </c>
       <c r="L20">
-        <v>265.02227783203125</v>
+        <v>358.8104248046875</v>
       </c>
       <c r="M20">
-        <v>265.02227783203125</v>
+        <v>358.8104248046875</v>
       </c>
       <c r="N20">
-        <v>0</v>
+        <v>199.25689697265625</v>
       </c>
       <c r="O20">
-        <v>0</v>
+        <v>199.25689697265625</v>
       </c>
       <c r="P20">
-        <v>265.02227783203125</v>
+        <v>1127.50244140625</v>
       </c>
       <c r="Q20">
-        <v>265.02227783203125</v>
+        <v>1127.50244140625</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -1383,43 +1335,43 @@
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="E21">
-        <v>4.8000000000000001E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="F21">
-        <v>4.8000000000000001E-2</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="G21">
-        <v>4.8000000000000001E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="H21">
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="I21">
-        <v>4.7E-2</v>
+        <v>0.05</v>
       </c>
       <c r="J21">
-        <v>4.7E-2</v>
+        <v>0.23799999999999999</v>
       </c>
       <c r="K21">
-        <v>4.7E-2</v>
+        <v>0.24199999999999999</v>
       </c>
       <c r="L21">
-        <v>2932.18994140625</v>
+        <v>3148.040771484375</v>
       </c>
       <c r="M21">
-        <v>2837.3031616210938</v>
+        <v>3098.0606079101563</v>
       </c>
       <c r="N21">
-        <v>0</v>
+        <v>174.407958984375</v>
       </c>
       <c r="O21">
-        <v>0</v>
+        <v>352.39410400390625</v>
       </c>
       <c r="P21">
-        <v>2932.18994140625</v>
+        <v>3457.4203491210938</v>
       </c>
       <c r="Q21">
-        <v>2837.3031616210938</v>
+        <v>7521.0342407226563</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -1436,22 +1388,22 @@
         <v>1.6E-2</v>
       </c>
       <c r="I22">
-        <v>1.7000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="J22">
-        <v>1.7000000000000001E-2</v>
+        <v>0.185</v>
       </c>
       <c r="K22">
-        <v>1.7000000000000001E-2</v>
+        <v>0.189</v>
       </c>
       <c r="M22">
-        <v>7.1563720703125</v>
+        <v>26.78680419921875</v>
       </c>
       <c r="O22">
-        <v>0</v>
+        <v>24.6429443359375</v>
       </c>
       <c r="Q22">
-        <v>7.1563720703125</v>
+        <v>702.81219482421875</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -1468,43 +1420,19 @@
         <v>3.1E-2</v>
       </c>
       <c r="E23">
-        <v>6.5000000000000002E-2</v>
-      </c>
-      <c r="F23">
-        <v>6.5000000000000002E-2</v>
-      </c>
-      <c r="G23">
-        <v>6.5000000000000002E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="H23">
         <v>3.1E-2</v>
       </c>
       <c r="I23">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="J23">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="K23">
-        <v>6.4000000000000001E-2</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="L23">
-        <v>3773.895263671875</v>
+        <v>3870.6436157226563</v>
       </c>
       <c r="M23">
-        <v>3732.5210571289063</v>
-      </c>
-      <c r="N23">
-        <v>0</v>
-      </c>
-      <c r="O23">
-        <v>0</v>
-      </c>
-      <c r="P23">
-        <v>3773.895263671875</v>
-      </c>
-      <c r="Q23">
-        <v>3732.5210571289063</v>
+        <v>3845.8786010742188</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -1521,43 +1449,31 @@
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="E24">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="F24">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="G24">
-        <v>5.1999999999999998E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="H24">
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="I24">
-        <v>3.5000000000000003E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="J24">
-        <v>3.5000000000000003E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="K24">
-        <v>3.5000000000000003E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="L24">
-        <v>931.58721923828125</v>
+        <v>1082.6034545898438</v>
       </c>
       <c r="M24">
-        <v>57.342529296875</v>
-      </c>
-      <c r="N24">
-        <v>0</v>
+        <v>223.50311279296875</v>
       </c>
       <c r="O24">
-        <v>0</v>
-      </c>
-      <c r="P24">
-        <v>931.58721923828125</v>
+        <v>220.245361328125</v>
       </c>
       <c r="Q24">
-        <v>57.342529296875</v>
+        <v>575.5157470703125</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -1574,43 +1490,19 @@
         <v>2.7E-2</v>
       </c>
       <c r="E25">
-        <v>3.3000000000000002E-2</v>
-      </c>
-      <c r="F25">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="G25">
-        <v>5.5E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="H25">
         <v>2.7E-2</v>
       </c>
       <c r="I25">
-        <v>3.3000000000000002E-2</v>
-      </c>
-      <c r="J25">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="K25">
-        <v>5.5E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="L25">
-        <v>43.22052001953125</v>
+        <v>290.85540771484375</v>
       </c>
       <c r="M25">
-        <v>43.22052001953125</v>
-      </c>
-      <c r="N25">
-        <v>221.160888671875</v>
-      </c>
-      <c r="O25">
-        <v>221.160888671875</v>
-      </c>
-      <c r="P25">
-        <v>276.02386474609375</v>
-      </c>
-      <c r="Q25">
-        <v>276.02386474609375</v>
+        <v>290.85540771484375</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
@@ -1627,43 +1519,43 @@
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="E26">
-        <v>5.0999999999999997E-2</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="F26">
-        <v>5.0999999999999997E-2</v>
+        <v>0.218</v>
       </c>
       <c r="G26">
-        <v>5.0999999999999997E-2</v>
+        <v>0.22700000000000001</v>
       </c>
       <c r="H26">
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="I26">
-        <v>5.0999999999999997E-2</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="J26">
-        <v>5.0999999999999997E-2</v>
+        <v>0.222</v>
       </c>
       <c r="K26">
-        <v>5.0999999999999997E-2</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="L26">
-        <v>1362.7243041992188</v>
+        <v>1475.067138671875</v>
       </c>
       <c r="M26">
-        <v>1362.7243041992188</v>
+        <v>1475.067138671875</v>
       </c>
       <c r="N26">
-        <v>0</v>
+        <v>456.390380859375</v>
       </c>
       <c r="O26">
-        <v>0</v>
+        <v>184.600830078125</v>
       </c>
       <c r="P26">
-        <v>1362.7243041992188</v>
+        <v>3544.43359375</v>
       </c>
       <c r="Q26">
-        <v>1362.7243041992188</v>
+        <v>3407.9513549804688</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
@@ -1680,31 +1572,19 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="E27">
-        <v>0.06</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="H27">
         <v>3.1E-2</v>
       </c>
       <c r="I27">
-        <v>6.0999999999999999E-2</v>
-      </c>
-      <c r="J27">
-        <v>6.0999999999999999E-2</v>
-      </c>
-      <c r="K27">
-        <v>6.0999999999999999E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="L27">
-        <v>2300.1861572265625</v>
+        <v>2347.2061157226563</v>
       </c>
       <c r="M27">
-        <v>2564.3234252929688</v>
-      </c>
-      <c r="O27">
-        <v>0</v>
-      </c>
-      <c r="Q27">
-        <v>2564.3234252929688</v>
+        <v>2721.37451171875</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -1721,43 +1601,43 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="E28">
-        <v>4.8000000000000001E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="F28">
-        <v>4.8000000000000001E-2</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="G28">
-        <v>4.8000000000000001E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="H28">
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="I28">
-        <v>4.8000000000000001E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="J28">
-        <v>4.8000000000000001E-2</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="K28">
-        <v>4.8000000000000001E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="L28">
-        <v>4629.4708251953125</v>
+        <v>4911.6744995117188</v>
       </c>
       <c r="M28">
-        <v>4585.8688354492188</v>
+        <v>4868.072509765625</v>
       </c>
       <c r="N28">
-        <v>0</v>
+        <v>162.22381591796875</v>
       </c>
       <c r="O28">
-        <v>0</v>
+        <v>135.30731201171875</v>
       </c>
       <c r="P28">
-        <v>4629.4708251953125</v>
+        <v>5159.1110229492188</v>
       </c>
       <c r="Q28">
-        <v>4585.8688354492188</v>
+        <v>5088.592529296875</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -1774,31 +1654,31 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="E29">
-        <v>5.2999999999999999E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="F29">
-        <v>5.2999999999999999E-2</v>
+        <v>0.14099999999999999</v>
       </c>
       <c r="G29">
-        <v>5.2999999999999999E-2</v>
+        <v>0.14899999999999999</v>
       </c>
       <c r="H29">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="I29">
-        <v>5.0999999999999997E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="L29">
-        <v>982.69462585449219</v>
+        <v>1112.7138137817383</v>
       </c>
       <c r="M29">
-        <v>902.68611907958984</v>
+        <v>938.75885009765625</v>
       </c>
       <c r="N29">
-        <v>0</v>
+        <v>288.848876953125</v>
       </c>
       <c r="P29">
-        <v>982.69462585449219</v>
+        <v>2259.4547271728516</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -1815,43 +1695,43 @@
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="E30">
-        <v>4.5999999999999999E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="F30">
-        <v>4.5999999999999999E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="G30">
-        <v>4.5999999999999999E-2</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="H30">
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="I30">
-        <v>4.5999999999999999E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="J30">
-        <v>4.5999999999999999E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="K30">
-        <v>4.5999999999999999E-2</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="L30">
-        <v>523.79608154296875</v>
+        <v>553.1463623046875</v>
       </c>
       <c r="M30">
-        <v>523.79608154296875</v>
+        <v>553.1463623046875</v>
       </c>
       <c r="N30">
-        <v>0</v>
+        <v>571.0601806640625</v>
       </c>
       <c r="O30">
-        <v>0</v>
+        <v>579.52117919921875</v>
       </c>
       <c r="P30">
-        <v>523.79608154296875</v>
+        <v>1144.0811157226563</v>
       </c>
       <c r="Q30">
-        <v>523.79608154296875</v>
+        <v>1144.0811157226563</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -1879,43 +1759,43 @@
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="E32">
-        <v>3.9E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="F32">
-        <v>3.9E-2</v>
+        <v>0.112</v>
       </c>
       <c r="G32">
-        <v>3.9E-2</v>
+        <v>0.11600000000000001</v>
       </c>
       <c r="H32">
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="I32">
-        <v>0.04</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="J32">
-        <v>0.04</v>
+        <v>0.112</v>
       </c>
       <c r="K32">
-        <v>0.04</v>
+        <v>0.11600000000000001</v>
       </c>
       <c r="L32">
-        <v>26.06201171875</v>
+        <v>51.85699462890625</v>
       </c>
       <c r="M32">
-        <v>35.2325439453125</v>
+        <v>58.50982666015625</v>
       </c>
       <c r="N32">
-        <v>0</v>
+        <v>47.85919189453125</v>
       </c>
       <c r="O32">
-        <v>0</v>
+        <v>47.85919189453125</v>
       </c>
       <c r="P32">
-        <v>26.06201171875</v>
+        <v>334.1522216796875</v>
       </c>
       <c r="Q32">
-        <v>35.2325439453125</v>
+        <v>334.1522216796875</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
@@ -1932,31 +1812,19 @@
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="E33">
-        <v>3.9E-2</v>
-      </c>
-      <c r="F33">
-        <v>0.04</v>
-      </c>
-      <c r="G33">
-        <v>4.1000000000000002E-2</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="H33">
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="I33">
-        <v>3.7999999999999999E-2</v>
+        <v>3.9E-2</v>
       </c>
       <c r="L33">
+        <v>92.09442138671875</v>
+      </c>
+      <c r="M33">
         <v>63.28582763671875</v>
-      </c>
-      <c r="M33">
-        <v>56.34307861328125</v>
-      </c>
-      <c r="N33">
-        <v>7.3089599609375</v>
-      </c>
-      <c r="P33">
-        <v>77.239990234375</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
@@ -1973,43 +1841,19 @@
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="E34">
-        <v>0.05</v>
-      </c>
-      <c r="F34">
-        <v>0.05</v>
-      </c>
-      <c r="G34">
-        <v>0.05</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="H34">
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="I34">
-        <v>0.05</v>
-      </c>
-      <c r="J34">
-        <v>0.05</v>
-      </c>
-      <c r="K34">
-        <v>0.05</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="L34">
-        <v>5352.783203125</v>
+        <v>6103.5079956054688</v>
       </c>
       <c r="M34">
-        <v>5352.783203125</v>
-      </c>
-      <c r="N34">
-        <v>0</v>
-      </c>
-      <c r="O34">
-        <v>0</v>
-      </c>
-      <c r="P34">
-        <v>5352.783203125</v>
-      </c>
-      <c r="Q34">
-        <v>5352.783203125</v>
+        <v>6103.5079956054688</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
@@ -2026,43 +1870,43 @@
         <v>0.04</v>
       </c>
       <c r="E35">
-        <v>0.05</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="F35">
-        <v>0.05</v>
+        <v>0.153</v>
       </c>
       <c r="G35">
-        <v>0.05</v>
+        <v>0.161</v>
       </c>
       <c r="H35">
         <v>0.04</v>
       </c>
       <c r="I35">
-        <v>0.05</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="J35">
-        <v>0.05</v>
+        <v>0.153</v>
       </c>
       <c r="K35">
-        <v>0.05</v>
+        <v>0.161</v>
       </c>
       <c r="L35">
-        <v>1658.660888671875</v>
+        <v>1977.5161743164063</v>
       </c>
       <c r="M35">
-        <v>1658.660888671875</v>
+        <v>1977.5161743164063</v>
       </c>
       <c r="N35">
-        <v>0</v>
+        <v>817.9931640625</v>
       </c>
       <c r="O35">
-        <v>0</v>
+        <v>817.9931640625</v>
       </c>
       <c r="P35">
-        <v>1658.660888671875</v>
+        <v>5155.6777954101563</v>
       </c>
       <c r="Q35">
-        <v>1658.660888671875</v>
+        <v>5155.6777954101563</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
@@ -2079,43 +1923,19 @@
         <v>0.03</v>
       </c>
       <c r="E36">
-        <v>5.5E-2</v>
-      </c>
-      <c r="F36">
-        <v>5.5E-2</v>
-      </c>
-      <c r="G36">
-        <v>5.5E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="H36">
         <v>0.03</v>
       </c>
       <c r="I36">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="J36">
-        <v>0.06</v>
-      </c>
-      <c r="K36">
-        <v>0.06</v>
+        <v>6.3E-2</v>
       </c>
       <c r="L36">
-        <v>1205.108642578125</v>
+        <v>1303.6117553710938</v>
       </c>
       <c r="M36">
-        <v>1303.6117553710938</v>
-      </c>
-      <c r="N36">
-        <v>0</v>
-      </c>
-      <c r="O36">
-        <v>0</v>
-      </c>
-      <c r="P36">
-        <v>1205.108642578125</v>
-      </c>
-      <c r="Q36">
-        <v>1339.6377563476563</v>
+        <v>1409.5840454101563</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
@@ -2132,43 +1952,31 @@
         <v>0.06</v>
       </c>
       <c r="E37">
-        <v>0.06</v>
+        <v>6.3E-2</v>
       </c>
       <c r="F37">
-        <v>0.06</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="G37">
-        <v>0.06</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="H37">
         <v>0.124</v>
       </c>
       <c r="I37">
-        <v>0.124</v>
-      </c>
-      <c r="J37">
-        <v>0.124</v>
-      </c>
-      <c r="K37">
-        <v>0.124</v>
+        <v>0.127</v>
       </c>
       <c r="L37">
-        <v>0</v>
+        <v>51.8341064453125</v>
       </c>
       <c r="M37">
-        <v>0</v>
+        <v>57.74688720703125</v>
       </c>
       <c r="N37">
-        <v>0</v>
-      </c>
-      <c r="O37">
-        <v>0</v>
+        <v>54.2755126953125</v>
       </c>
       <c r="P37">
-        <v>0</v>
-      </c>
-      <c r="Q37">
-        <v>0</v>
+        <v>200.00457763671875</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
@@ -2185,43 +1993,19 @@
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="E38">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="F38">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="G38">
-        <v>3.5000000000000003E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="H38">
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="I38">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="J38">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="K38">
-        <v>3.5000000000000003E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="L38">
-        <v>11.138916015625</v>
+        <v>41.35894775390625</v>
       </c>
       <c r="M38">
-        <v>11.138916015625</v>
-      </c>
-      <c r="N38">
-        <v>0</v>
-      </c>
-      <c r="O38">
-        <v>0</v>
-      </c>
-      <c r="P38">
-        <v>11.138916015625</v>
-      </c>
-      <c r="Q38">
-        <v>11.138916015625</v>
+        <v>41.35894775390625</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -2238,19 +2022,19 @@
         <v>3.9E-2</v>
       </c>
       <c r="E39">
-        <v>4.5999999999999999E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="H39">
         <v>3.9E-2</v>
       </c>
       <c r="I39">
-        <v>4.5999999999999999E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="L39">
-        <v>113.76190185546875</v>
+        <v>169.8760986328125</v>
       </c>
       <c r="M39">
-        <v>113.76190185546875</v>
+        <v>169.8760986328125</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
@@ -2267,43 +2051,19 @@
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="E40">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="F40">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="G40">
-        <v>4.8000000000000001E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="H40">
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="I40">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="J40">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="K40">
-        <v>4.8000000000000001E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="L40">
-        <v>3570.5337524414063</v>
+        <v>3780.5404663085938</v>
       </c>
       <c r="M40">
-        <v>3570.5337524414063</v>
-      </c>
-      <c r="N40">
-        <v>0</v>
-      </c>
-      <c r="O40">
-        <v>0</v>
-      </c>
-      <c r="P40">
-        <v>3570.5337524414063</v>
-      </c>
-      <c r="Q40">
-        <v>3570.5337524414063</v>
+        <v>3780.5404663085938</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
@@ -2320,43 +2080,19 @@
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="E41">
-        <v>6.8000000000000005E-2</v>
-      </c>
-      <c r="F41">
-        <v>6.8000000000000005E-2</v>
-      </c>
-      <c r="G41">
-        <v>6.8000000000000005E-2</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="H41">
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="I41">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="J41">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="K41">
-        <v>6.9000000000000006E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="L41">
-        <v>5845.1309204101563</v>
+        <v>5965.576171875</v>
       </c>
       <c r="M41">
-        <v>5887.9776000976563</v>
-      </c>
-      <c r="N41">
-        <v>0</v>
-      </c>
-      <c r="O41">
-        <v>0</v>
-      </c>
-      <c r="P41">
-        <v>5845.1309204101563</v>
-      </c>
-      <c r="Q41">
-        <v>5887.9776000976563</v>
+        <v>5998.3673095703125</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
@@ -2373,19 +2109,19 @@
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="E42">
-        <v>3.7999999999999999E-2</v>
+        <v>3.9E-2</v>
       </c>
       <c r="H42">
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="I42">
-        <v>4.1000000000000002E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="L42">
-        <v>1376.2588500976563</v>
+        <v>1437.2100830078125</v>
       </c>
       <c r="M42">
-        <v>1554.4586181640625</v>
+        <v>1608.4136962890625</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
@@ -2402,43 +2138,43 @@
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="E43">
-        <v>5.3999999999999999E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="F43">
-        <v>5.3999999999999999E-2</v>
+        <v>0.22600000000000001</v>
       </c>
       <c r="G43">
-        <v>5.3999999999999999E-2</v>
+        <v>0.23</v>
       </c>
       <c r="H43">
         <v>0.04</v>
       </c>
       <c r="I43">
-        <v>5.3999999999999999E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="J43">
-        <v>5.3999999999999999E-2</v>
+        <v>0.185</v>
       </c>
       <c r="K43">
-        <v>5.3999999999999999E-2</v>
+        <v>0.188</v>
       </c>
       <c r="L43">
-        <v>1767.6162719726563</v>
+        <v>2086.0977172851563</v>
       </c>
       <c r="M43">
-        <v>1854.2556762695313</v>
+        <v>2172.7371215820313</v>
       </c>
       <c r="N43">
-        <v>0</v>
+        <v>430.22918701171875</v>
       </c>
       <c r="O43">
-        <v>0</v>
+        <v>239.81475830078125</v>
       </c>
       <c r="P43">
-        <v>1767.6162719726563</v>
+        <v>8755.7296752929688</v>
       </c>
       <c r="Q43">
-        <v>1854.2556762695313</v>
+        <v>6192.0166015625</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
@@ -2455,43 +2191,43 @@
         <v>2.3E-2</v>
       </c>
       <c r="E44">
-        <v>3.6999999999999998E-2</v>
+        <v>0.04</v>
       </c>
       <c r="F44">
-        <v>3.6999999999999998E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="G44">
-        <v>3.6999999999999998E-2</v>
+        <v>7.8E-2</v>
       </c>
       <c r="H44">
         <v>2.3E-2</v>
       </c>
       <c r="I44">
-        <v>3.6999999999999998E-2</v>
+        <v>0.04</v>
       </c>
       <c r="J44">
-        <v>3.6999999999999998E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="K44">
-        <v>3.6999999999999998E-2</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="L44">
-        <v>295.806884765625</v>
+        <v>336.9293212890625</v>
       </c>
       <c r="M44">
-        <v>295.806884765625</v>
+        <v>336.9293212890625</v>
       </c>
       <c r="N44">
-        <v>0</v>
+        <v>184.71527099609375</v>
       </c>
       <c r="O44">
-        <v>0</v>
+        <v>224.884033203125</v>
       </c>
       <c r="P44">
-        <v>295.806884765625</v>
+        <v>596.1761474609375</v>
       </c>
       <c r="Q44">
-        <v>295.806884765625</v>
+        <v>636.34490966796875</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
@@ -2508,43 +2244,43 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="E45">
-        <v>2.4E-2</v>
+        <v>2.7E-2</v>
       </c>
       <c r="F45">
-        <v>2.4E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G45">
-        <v>2.4E-2</v>
+        <v>0.05</v>
       </c>
       <c r="H45">
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="I45">
-        <v>2.4E-2</v>
+        <v>2.7E-2</v>
       </c>
       <c r="J45">
-        <v>2.4E-2</v>
+        <v>0.03</v>
       </c>
       <c r="K45">
-        <v>2.4E-2</v>
+        <v>0.05</v>
       </c>
       <c r="L45">
-        <v>151.9927978515625</v>
+        <v>189.02587890625</v>
       </c>
       <c r="M45">
-        <v>162.66632080078125</v>
+        <v>199.69940185546875</v>
       </c>
       <c r="N45">
-        <v>0</v>
+        <v>552.80303955078125</v>
       </c>
       <c r="O45">
-        <v>0</v>
+        <v>552.80303955078125</v>
       </c>
       <c r="P45">
-        <v>151.9927978515625</v>
+        <v>758.9111328125</v>
       </c>
       <c r="Q45">
-        <v>162.66632080078125</v>
+        <v>769.58465576171875</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
@@ -2561,43 +2297,19 @@
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="E46">
-        <v>6.7000000000000004E-2</v>
-      </c>
-      <c r="F46">
-        <v>6.7000000000000004E-2</v>
-      </c>
-      <c r="G46">
-        <v>6.7000000000000004E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="H46">
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="I46">
-        <v>6.7000000000000004E-2</v>
-      </c>
-      <c r="J46">
-        <v>6.7000000000000004E-2</v>
-      </c>
-      <c r="K46">
-        <v>6.7000000000000004E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="L46">
-        <v>2706.756591796875</v>
+        <v>2745.2621459960938</v>
       </c>
       <c r="M46">
-        <v>2706.756591796875</v>
-      </c>
-      <c r="N46">
-        <v>0</v>
-      </c>
-      <c r="O46">
-        <v>0</v>
-      </c>
-      <c r="P46">
-        <v>2706.756591796875</v>
-      </c>
-      <c r="Q46">
-        <v>2706.756591796875</v>
+        <v>2745.2621459960938</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
@@ -2614,43 +2326,43 @@
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="E47">
-        <v>4.3999999999999997E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="F47">
-        <v>4.3999999999999997E-2</v>
+        <v>0.05</v>
       </c>
       <c r="G47">
-        <v>4.3999999999999997E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="H47">
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="I47">
-        <v>4.3999999999999997E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="J47">
-        <v>4.3999999999999997E-2</v>
+        <v>0.05</v>
       </c>
       <c r="K47">
-        <v>4.3999999999999997E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="L47">
-        <v>0</v>
+        <v>80.72662353515625</v>
       </c>
       <c r="M47">
-        <v>0</v>
+        <v>80.72662353515625</v>
       </c>
       <c r="N47">
-        <v>0</v>
+        <v>74.39422607421875</v>
       </c>
       <c r="O47">
-        <v>0</v>
+        <v>74.39422607421875</v>
       </c>
       <c r="P47">
-        <v>0</v>
+        <v>207.34405517578125</v>
       </c>
       <c r="Q47">
-        <v>0</v>
+        <v>207.34405517578125</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
@@ -2667,31 +2379,19 @@
         <v>6.2E-2</v>
       </c>
       <c r="E48">
-        <v>7.6999999999999999E-2</v>
-      </c>
-      <c r="F48">
-        <v>7.6999999999999999E-2</v>
-      </c>
-      <c r="G48">
-        <v>7.6999999999999999E-2</v>
+        <v>0.08</v>
       </c>
       <c r="H48">
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="I48">
-        <v>0.08</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="L48">
-        <v>101.32598876953125</v>
+        <v>119.293212890625</v>
       </c>
       <c r="M48">
-        <v>125.51116943359375</v>
-      </c>
-      <c r="N48">
-        <v>0</v>
-      </c>
-      <c r="P48">
-        <v>101.32598876953125</v>
+        <v>136.1846923828125</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
@@ -2708,43 +2408,43 @@
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="E49">
-        <v>4.8000000000000001E-2</v>
+        <v>0.05</v>
       </c>
       <c r="F49">
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="G49">
-        <v>6.2E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="H49">
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="I49">
-        <v>4.8000000000000001E-2</v>
+        <v>0.05</v>
       </c>
       <c r="J49">
         <v>5.5E-2</v>
       </c>
       <c r="K49">
-        <v>6.2E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="L49">
-        <v>1293.9300537109375</v>
+        <v>1338.3560180664063</v>
       </c>
       <c r="M49">
-        <v>1293.9300537109375</v>
+        <v>1338.3560180664063</v>
       </c>
       <c r="N49">
-        <v>171.5240478515625</v>
+        <v>222.35870361328125</v>
       </c>
       <c r="O49">
-        <v>154.7393798828125</v>
+        <v>205.57403564453125</v>
       </c>
       <c r="P49">
-        <v>1569.4656372070313</v>
+        <v>1620.30029296875</v>
       </c>
       <c r="Q49">
-        <v>1569.4656372070313</v>
+        <v>1620.30029296875</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
@@ -2772,43 +2472,19 @@
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="E51">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="F51">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="G51">
-        <v>5.3999999999999999E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="H51">
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="I51">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="J51">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="K51">
-        <v>5.3999999999999999E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="L51">
-        <v>1959.2666625976563</v>
+        <v>2057.6248168945313</v>
       </c>
       <c r="M51">
-        <v>1959.2666625976563</v>
-      </c>
-      <c r="N51">
-        <v>0</v>
-      </c>
-      <c r="O51">
-        <v>0</v>
-      </c>
-      <c r="P51">
-        <v>1959.2666625976563</v>
-      </c>
-      <c r="Q51">
-        <v>1959.2666625976563</v>
+        <v>2057.6248168945313</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
@@ -2836,43 +2512,43 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="E53">
-        <v>5.5E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="F53">
-        <v>5.5E-2</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="G53">
-        <v>5.5E-2</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="H53">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="I53">
-        <v>5.5E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="J53">
-        <v>5.5E-2</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="K53">
-        <v>5.5E-2</v>
+        <v>0.111</v>
       </c>
       <c r="L53">
-        <v>4064.5904541015625</v>
+        <v>4233.2305908203125</v>
       </c>
       <c r="M53">
-        <v>4064.5904541015625</v>
+        <v>4233.2305908203125</v>
       </c>
       <c r="N53">
-        <v>0</v>
+        <v>308.4259033203125</v>
       </c>
       <c r="O53">
-        <v>0</v>
+        <v>1646.1257934570313</v>
       </c>
       <c r="P53">
-        <v>4064.5904541015625</v>
+        <v>4657.5241088867188</v>
       </c>
       <c r="Q53">
-        <v>4064.5904541015625</v>
+        <v>6749.5651245117188</v>
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.25">
@@ -2889,43 +2565,43 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="E54">
-        <v>4.9000000000000002E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="F54">
         <v>6.3E-2</v>
       </c>
       <c r="G54">
-        <v>6.3E-2</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="H54">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="I54">
-        <v>4.8000000000000001E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="J54">
-        <v>4.8000000000000001E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="K54">
-        <v>4.8000000000000001E-2</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="L54">
-        <v>1488.7924194335938</v>
+        <v>1513.2064819335938</v>
       </c>
       <c r="M54">
-        <v>1468.1549072265625</v>
+        <v>1513.2064819335938</v>
       </c>
       <c r="N54">
-        <v>0</v>
+        <v>29.693603515625</v>
       </c>
       <c r="O54">
-        <v>0</v>
+        <v>73.58551025390625</v>
       </c>
       <c r="P54">
-        <v>1601.837158203125</v>
+        <v>1631.53076171875</v>
       </c>
       <c r="Q54">
-        <v>1468.1549072265625</v>
+        <v>1754.1427612304688</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.25">
@@ -2942,43 +2618,43 @@
         <v>3.9E-2</v>
       </c>
       <c r="E55">
-        <v>4.2999999999999997E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="F55">
-        <v>4.2999999999999997E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="G55">
-        <v>4.2999999999999997E-2</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="H55">
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="I55">
-        <v>6.0999999999999999E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="J55">
-        <v>6.0999999999999999E-2</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="K55">
-        <v>6.0999999999999999E-2</v>
+        <v>0.13600000000000001</v>
       </c>
       <c r="L55">
-        <v>122.0703125</v>
+        <v>214.17236328125</v>
       </c>
       <c r="M55">
-        <v>202.6519775390625</v>
+        <v>309.53216552734375</v>
       </c>
       <c r="N55">
-        <v>0</v>
+        <v>499.83978271484375</v>
       </c>
       <c r="O55">
-        <v>0</v>
+        <v>104.8431396484375</v>
       </c>
       <c r="P55">
-        <v>122.0703125</v>
+        <v>834.5947265625</v>
       </c>
       <c r="Q55">
-        <v>202.6519775390625</v>
+        <v>1475.8377075195313</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.25">
@@ -2995,43 +2671,43 @@
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="E56">
-        <v>3.3000000000000002E-2</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="F56">
-        <v>3.3000000000000002E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="G56">
-        <v>3.3000000000000002E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="H56">
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="I56">
-        <v>3.3000000000000002E-2</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="J56">
-        <v>3.3000000000000002E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="K56">
-        <v>3.3000000000000002E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="L56">
-        <v>74.615478515625</v>
+        <v>100.30364990234375</v>
       </c>
       <c r="M56">
-        <v>74.615478515625</v>
+        <v>100.30364990234375</v>
       </c>
       <c r="N56">
-        <v>0</v>
+        <v>88.60015869140625</v>
       </c>
       <c r="O56">
-        <v>0</v>
+        <v>88.60015869140625</v>
       </c>
       <c r="P56">
-        <v>74.615478515625</v>
+        <v>208.770751953125</v>
       </c>
       <c r="Q56">
-        <v>74.615478515625</v>
+        <v>208.770751953125</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.25">
@@ -3048,22 +2724,22 @@
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="I57">
-        <v>2.7E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J57">
-        <v>2.7E-2</v>
+        <v>0.05</v>
       </c>
       <c r="K57">
-        <v>2.7E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="M57">
-        <v>6.77490234375</v>
+        <v>25.12359619140625</v>
       </c>
       <c r="O57">
-        <v>0</v>
+        <v>17.23480224609375</v>
       </c>
       <c r="Q57">
-        <v>6.77490234375</v>
+        <v>102.08892822265625</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
@@ -3080,19 +2756,19 @@
         <v>0.04</v>
       </c>
       <c r="E58">
-        <v>4.7E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="H58">
         <v>0.04</v>
       </c>
       <c r="I58">
-        <v>4.7E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="L58">
-        <v>451.3092041015625</v>
+        <v>554.19921875</v>
       </c>
       <c r="M58">
-        <v>451.3092041015625</v>
+        <v>554.19921875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>